<commit_message>
added automatic code for velocity groundTruth
</commit_message>
<xml_diff>
--- a/geometryVelocity.xlsx
+++ b/geometryVelocity.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utente\Documents\GitHub\ESM-based-NAH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utente\Documents\GitHub\ESM-based-NAH-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>bottom</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>center point [inches]</t>
-  </si>
-  <si>
-    <t>8,,3</t>
   </si>
   <si>
     <t>YY</t>
@@ -468,7 +465,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:P5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,8 +705,8 @@
       <c r="B7" s="2">
         <v>5.9</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
+      <c r="C7" s="2">
+        <v>8.3000000000000007</v>
       </c>
       <c r="D7" s="2">
         <v>5.8</v>
@@ -743,7 +740,7 @@
       </c>
       <c r="C8" s="8">
         <f t="shared" si="0"/>
-        <v>211.45499999999998</v>
+        <v>211.32799999999995</v>
       </c>
       <c r="D8" s="8">
         <f t="shared" si="0"/>
@@ -791,7 +788,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="3">
         <f>+-2</f>
@@ -804,7 +801,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K13" s="3">
         <f>-6</f>

</xml_diff>